<commit_message>
Continued reading chapter 9 'Experiments' of 'Researching Information Systems and Computing'. The independent variable affects one or more dependent variables. The more independent variables are measures, the more complex the required statistical analysis. Experiments are used to show that one factor only causes an observed change. Different ways on controlling variables that might influence the outcome: Eliminate the factor from the experiment. Hold the factor constant. Use random selection of subjects. Use control groups. Make the researchers and subjects blind. Typical things which are observed and measured are mentioned on page 130. Apply a pre- and post-test for your experiment. Proxy measurements techniques might help if you cannot measure one variable directly. Many measures are related to each other. Decide beforehand what you want to measure.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD506197-4C6C-FB4A-801E-5F399D415E56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5563CE86-0BAB-4740-86B2-69D089AAEEC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -514,7 +514,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -564,7 +564,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>

<commit_message>
Started reading 'The Passionate Programmer' by Chad Fowler. Read the following chapters: 1. Lead or bleed? 2. Suppy and demand 3. Coding do not cut it anymore. 4. Be the worst 5. Invest in your intelligence 6. Do not listen to your parents. 7. Be a generalist 8. Be a specialist 9. Do not put all your eggs in someone elses basket 10. Love it or leave it 11. Learn to fish 12. Learn how businesses really work 13. Find a mentor 14. Be a mentor 15. Practice, practice, pratice 16. The way that you do it 17. On the shoulders of giants 18. Automate yourself into a job 19. Right now 20. Mind Reader 21. Daily Hit
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687DBBDD-E51A-9E40-BDC1-20F24D3EC0D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B618BAC-6E44-B843-B374-F88F3270C36A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Books to read</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Total page count</t>
+  </si>
+  <si>
+    <t>The Passionate Programmer: Creating a Remarkable Career in Software Development</t>
+  </si>
+  <si>
+    <t>Chad Fowler</t>
   </si>
 </sst>
 </file>
@@ -458,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D9D6FD-C1AC-2947-87E8-CDC23DD828D6}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -514,7 +520,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>772</v>
+        <v>861</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -576,6 +582,17 @@
       </c>
       <c r="C12">
         <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started reading Chapter 10 'Case Studies' of 'Researching Information Systems and Computing'. A case study looks at the chosen case within its real-life context. A case study approach does not test hypotheses. Case study teaching is not case study research. There are three basic types of case studies, namely exploratory, descriptive and explanatory study.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B22DF6-2336-1448-A50B-ED8A2E25838C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88D5E08-BCD4-894A-8B23-42FBC2601CA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -520,7 +520,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>885</v>
+        <v>888</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -570,7 +570,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>

<commit_message>
Continued reading 'The Passionate Programmer' by Chad Fowler. 22. Remember who you work for. 23. Be where you are at. 24. How good a job can i do today? 25. How much are you worth? 26. A pebble in a bucket of water. 27. Learn to love maintenance. 28. Eight-hour burn. 29. Learn how to fail. 30. Say 'No'. 31. Do not panic. 32. Say it, do it, show it.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C6A3CA-EFBC-3F41-95E5-1187F171EA7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8071D81D-BC6F-F54B-8430-E84CF17EFF33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -520,7 +520,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>936</v>
+        <v>980</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -592,7 +592,7 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>89</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued reading 'The Passionate Programmer' by Chad Fowler. 39. Let your voice be heard -> Start a blog, write a book, contrinute to open source projects. 40. Build your brand -> Your name is your brand. Google never forgets. 41. Release your code -> Anyone can use Rails. Few can say Rails contributor. Contribute to open source projects. Release your own code or library. 42. Remarkability -> viral marketing. Purple cow example. Demo or die. Do not just master a subject - write a book about it. 43. Making the hang -> Fear gets between us and the pros. Extrovert Chris.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2B89F9-B829-F74D-A97E-869B622D7D55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADA35A7-122E-974C-A0C1-2AB136FCCE3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -520,7 +520,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1049</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -592,7 +592,7 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued reading chapter 3 'Cut Costs' of 'The Spirit of Kaizen' by Robert Maurer. The people who are best able to reduce the costs of the job are the people who are actually performing that job. The average american employee makes only one suggestion every six years, while the average japanese worker proposes 18 ideas every year. Cost controll step 1: offer small rewards or none at all. There are two basic types of motivation: intrinsic and extrinsic. People have an inner drive to do meaningful work; they want to be challenged and proud of what they do. An intelligent system of rewards known as 'positive reinforcement' can mold human behavior. The key is to make small rewards. The most commonly cited reason that people leave a job is because they feel underappreciated.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7481A8-D9E8-3845-B5FB-C05664DF29DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535F4906-5313-5F43-93B8-4B8CC0E9288A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1213</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -612,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued reading chapter 12 'Ethnography' of 'Researching Information Systems and Computing' by Briony J Oates. Ethnography means a description of peoples or cultures. The initial research question for an ethnographer can be summarized as: 'What is life like for these people?'. Different sizes of cultures, sub-cultures, normal-groups, class-rooms. The researcher is the research instrument. Critics say that the researcher is not detached and objective. Ethnographers tend to be based in the interpretive or critical paradigms, whereas their critics are usually based in the positivist paradigm. So much depends on the people in the culture being studied. There are no defined procedures for Ethnographers which makes it look 'unscientific'.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535F4906-5313-5F43-93B8-4B8CC0E9288A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1EC290-8009-7C45-A867-FBB29F5F6482}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1216</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -576,7 +576,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>

<commit_message>
Continued reading chapter 12 'Ethnography' of 'Researching Information Systems and Computing' by Briony J Oates. There are three types of ethnography, namely holistic, semiotic and critical schools. Holistic school = go native. Semiotic school = thick description. Critical school = Uncover what is hidden and unspoken. Ethnographers should make detailed field notes on substance, methodology and analysis. It is essential that you write field notes regularly, Do not worry about whether something is relevant, just write it down. The description of ethnographers should be standalone studies, therefore they do not have to generalize.Ethnography should produce a theory or serve as a test-bed for theories that have already been advanced, to see whether they hold true in a particular context.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A137A9-F086-5C4A-B30E-1B9D1441A158}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534A2B1B-1769-504E-B63F-479C2FD6EA2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1224</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -576,7 +576,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>

<commit_message>
Continued reading chapter 4 'Improve Quality' of 'The Spirit of Kaizen' by Robert Maurer. Toyota example and the andon rope. At each step of the assembly line, he places a rope called the andon cord. Instead going through the whole assembly line and checking the product at the end, you can now repait the equipment while it is still relatively easy to repair. Kaizen requires that we look for, and address, mistakes while they are still small. Unless you are committed to addressing small mistakes, you risk having your attention hijacked by very big problems. High-reliability organization (HRO). Their attention to small mistakes is an antidote to the poison of perfectionism. Instead of expecting staff members to be perfect, HROs require them to be transparent. If you make a mistake, tell us so that we can prevent a bigger problem. Fix the problem, not the blame. Once you are aware of these mental blindfolds, you can lift them out of the way and make it easier to see mistakes.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534A2B1B-1769-504E-B63F-479C2FD6EA2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE1BA64-B8BE-B543-AA70-33AC7CA6EE90}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1227</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -612,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued reading chapter 12 'Ethnography' of 'Researching Information Systems and Computing' by Briony J Oates. Reflexivity is concerned with the relationship between the researcher, the participants, and the research process. Tell/write about your personal experience, background, life so people can interpret your research better. Decide for yourself how much you want to tell people about yourself. Ethnographers cannot reproduce everything they saw, they constuct a partial account of a culture. Ethnographer rather write books instead of journals because then they are not restricted to a certain amount of pages. Does the phenomena exist outside of the ethnographers mind?
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE1BA64-B8BE-B543-AA70-33AC7CA6EE90}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BBE68B-E234-8B49-940B-E554AA86B056}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15900" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -576,7 +576,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>

<commit_message>
Finished reading chapter 13 'Interviews' of 'Researching Information Systems and Computing' by Briony J Oates. Internet-based interviews: Unless it is skype or something similar, the interview is a set of written questions and answers. You are probably losing the richness of gestures and facial expressions. You have to prove the identity of the interviewee. Online interviews can be cheaper. The establishment of good inter-personal relationship is questionable. The simplest form of online interviews is email or real-time chat. You can also try to get volunteers via newsgroups and mailing lists. You have to know the internet slang and emojis. Online interviews can be very demanding because people expect a quick response. Examples of Interviews in IS and Computing Research: CASE tools example, introduction of a new computer system, interview of web developers via email example. Advantages and disadvantages of evaluating interview-based research can be found on page 198 and 199.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B752755-9D94-7048-8C4A-67160BF72D49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B365FE7C-FF0A-EB45-8DC7-5AF9755FAC67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1373</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -576,7 +576,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>

<commit_message>
Continued reading 'Calculus made easy' by Silvanus Thompson. Chapter 6 'Sums, Differences, Products and Quotients'. Sums and differences y = u + v -> dy/dx = du/dx + dv/dx. Products y = u * v -> dy/dx = u * dv/dx + v * du/dx. Quotients y = u/v -> dy/dx = (v * du/dx - u * du/dx)/v^2. Chapter 7 'Successive Differentiation'. The corresponding symbol for the differential coefficient is f<apostrophe>(x) which is the same as dy/dx. First derivative: f<apostrophe>(x) same as dy/dx. Second derivative: f<two apostrophes>(x) same as d^2y/dx^2. Third derivative f<three apostrophes>(x) same as d^3y/dx^3.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E2983C-18F6-244D-93F0-62D2A28F3C2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6F49FC-AC9D-2F4A-A444-FB1288B4C929}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -529,7 +529,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1413</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -632,7 +632,7 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued reading chapter 14 'Observations'. Observations include looking, hearing, smelling, tasting and touching. Observations can be used with any other research strategy. You can also observe inanimate objects like software programs. Covert observation: people being observed do not know it. Overt observations: people know that they are being observed. When in doubt: use overt observation. Hawthorn effect: people modify their behavior because they know they are being observer.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6F49FC-AC9D-2F4A-A444-FB1288B4C929}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B522B782-9B5B-F845-BE80-C6ADE8DF6C4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -529,7 +529,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1431</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -582,7 +582,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:5">

</xml_diff>

<commit_message>
Finished reading chapter 13 'Other useful dodges' of 'Calculus made easy' by Silvanus Thompson. Differentiating a fraction can be difficult. To overcome this problem it is sometimes a good idea to split the fraction into two simpler fractions such that their sum is equivalent to the original fraction. It is important to mention that the examples in this chapter only apply to proper algebraic fractions, which have the numerator of a lesser degree than the denominator. (3x + 1)/(x^2 - 1) could be simplified to 1/(x + 1) * 2/(x - 1). Differential of an inverse function. Being given a function, if it be easier to differentiate the inverse function, this may be done, and the reciprocal of the differential coefficient of the inverse function gives the differential coefficient of the given function itself.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA34B22-B7FC-AE4F-96FF-4F970051A619}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3292B5-4CB1-D547-8A97-86C5692B4AA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -529,7 +529,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1500</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -632,7 +632,7 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>119</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued reading chapter 14 "On true compound interest and the law of organic growth" of "Calculus made easy" by Silvanus Thompson. The Die-away curve and the logarithmic curve. Exponential growth and decay: y(t) = a * e^(kt), where y(t) = value of time "t", a = value at the start, K = rate of growth (when greater than 0) or decay (when less than zero), t = time. Continued reading chapter 15 "How to deal with sines and cosines" of "Calculus made easy" by Silvanus Thompson. d/dx of sin(x) is cos(x), d/dx of cos(x) is -sin(x), d/dx of -sin(x) is -cos(x), d/dy of -cos(x) is sin(x). d/dx of tan(x) is sec^2(x) = 1 + tan^2(x) * 1/cos^2(x). Camp SohCahToa.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D615D1-92D8-BB42-9C57-8342DCDD6A84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EDF501-87FE-574D-BF08-9ADFE5832C98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -529,7 +529,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1533</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -632,7 +632,7 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>152</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished reading chapter 14 "Observations" of "Researching Information Systems and Computing" by Briony J Oates. Evaluating Observation-based Research. Advantages of systematic and participant observation can be found on page 214. Disadvantages of systematic and participant observation can be found on page 214 and 215. Evaluation guide for systematic observation can be found on page 215 and participant observation on page 216.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A149FA2-3EF1-334D-894A-5463CBD7F01C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4815407C-08F9-4E4F-92EE-67E22E76DECD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Books to read</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Silvanus Thompson</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence: Foundations of Computational Agents (2nd Edition)</t>
+  </si>
+  <si>
+    <t>David L. Poole and Alan K. Mackworth</t>
   </si>
 </sst>
 </file>
@@ -473,16 +479,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D9D6FD-C1AC-2947-87E8-CDC23DD828D6}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="90" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
@@ -529,7 +535,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1639</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -582,7 +588,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -636,6 +642,14 @@
       </c>
       <c r="D15" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished reading chapter 1 "How best to use this book" of "A Students Guide to Bayesian Statistics" by Ben Lambert. Prerequisites to read this book are an understanding of basic algebra and products and summations. Most of the examples are writting R and Stan. Suggested further reading for me: Bayesian Data Analysis. MCMC: Markov Chain Monte Carlo will be explained later on in the book.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4815407C-08F9-4E4F-92EE-67E22E76DECD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3254914E-E385-D641-AB0C-A018281EA353}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -535,7 +535,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1644</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -599,7 +599,7 @@
         <v>18</v>
       </c>
       <c r="C12">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5">

</xml_diff>

<commit_message>
Continued reading chapter 2 "The subjective worlds of frequentist and bayesian statistics" of "A students guide to bayesian statistics" by Ben Lambert. 3.1 - "Chapter Mission Statement". Purpose of statistical inference. Frequentist and bayesian inference. Bayes rule as an inversion process between cause and effect. 2.3 "Bayes rule - Allowing us to go from the effect back to its cause". Crooked casino and die roll example.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA0512D-728C-D348-A221-CE7E06B23C8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825B6D8B-E4A0-C84C-B67B-582299C64C50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -535,7 +535,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1630</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -599,7 +599,7 @@
         <v>18</v>
       </c>
       <c r="C12">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5">

</xml_diff>

<commit_message>
Finished reading "Make your own Neural Network" by Tariq Rashid. Creating your own feedforward network with one hidden layer to classifiy grayscale digits from the mnist dataset. Use vectorization technique and matrix multiplication in order to make the computation easier. Sigmoid activation function (scipy.special.expit) to involve non-linearity. Inputs times weights (add a bias), activate. Use the inverse of the expit function (logit) to reverse the prediction process and generate grayscale images from predictions. Backpropagation. How does gradient descent work exactly? How are the weights adjusted according to the error?
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825B6D8B-E4A0-C84C-B67B-582299C64C50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FFB1B2-12D0-B149-829F-D9FC1A77EDB4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Books to read</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>David L. Poole and Alan K. Mackworth</t>
+  </si>
+  <si>
+    <t>Make your own Neural Network / Neuronale Netze selbst programmieren</t>
+  </si>
+  <si>
+    <t>Tariq Rashid</t>
   </si>
 </sst>
 </file>
@@ -479,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D9D6FD-C1AC-2947-87E8-CDC23DD828D6}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -535,7 +541,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1631</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -652,6 +658,20 @@
         <v>26</v>
       </c>
       <c r="C16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>211</v>
+      </c>
+      <c r="D17" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started reading "Operating System Concepts" by Abraham Silberschatz. Purpose of an operating system is to manage resources. Interrupts. Different kinds of memory. Volatile vs non-volatilve. Device controllers and device drivers.
</commit_message>
<xml_diff>
--- a/PageCountSummary.xlsx
+++ b/PageCountSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschmidl/Study/books-to-read/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FFB1B2-12D0-B149-829F-D9FC1A77EDB4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F34E4C8-72E8-8747-8A14-D478694CD8A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15880" xr2:uid="{6B0161F9-090C-9042-81A3-43F466117C6E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Books to read</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Tariq Rashid</t>
+  </si>
+  <si>
+    <t>Operating System Concepts</t>
+  </si>
+  <si>
+    <t>Abraham Silberschatz et al</t>
   </si>
 </sst>
 </file>
@@ -485,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D9D6FD-C1AC-2947-87E8-CDC23DD828D6}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -541,7 +547,7 @@
       </c>
       <c r="E7">
         <f>SUM(C7:C35)</f>
-        <v>1842</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -673,6 +679,17 @@
       </c>
       <c r="D17" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>